<commit_message>
Foglio degli esperimenti personalizzato per Luca
</commit_message>
<xml_diff>
--- a/Relation Extraction - Experiments.xlsx
+++ b/Relation Extraction - Experiments.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.Maurici\Documents\Git_projects\Personal GitHub\relation-extraction\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715A4E4F-837C-49E9-AF6A-3D5FE89AB69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sveva Esperimenti" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Luca Esperimenti" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Livio Esperimenti" sheetId="3" r:id="rId6"/>
+    <sheet name="Sveva Esperimenti" sheetId="1" r:id="rId1"/>
+    <sheet name="Luca Esperimenti" sheetId="2" r:id="rId2"/>
+    <sheet name="Livio Esperimenti" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Dataset: Semeval task 8</t>
   </si>
@@ -91,48 +100,74 @@
   </si>
   <si>
     <t>Model (Relation Extraction Binary) - Dataset Non Bilanciato</t>
+  </si>
+  <si>
+    <t>f1 (train)</t>
+  </si>
+  <si>
+    <t>emb BERT + emb pretrained + emb NER cmpl + LSTM</t>
+  </si>
+  <si>
+    <t>embedding_dim_pretrained</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -140,7 +175,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -150,59 +185,76 @@
     </fill>
   </fills>
   <borders count="11">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -211,9 +263,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -222,11 +274,27 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -236,113 +304,80 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -532,30 +567,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="56.75"/>
-    <col customWidth="1" min="3" max="3" width="20.13"/>
-    <col customWidth="1" min="4" max="4" width="17.63"/>
-    <col customWidth="1" min="5" max="5" width="17.25"/>
+    <col min="2" max="2" width="56.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,22 +615,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4">
-        <v>2608.0</v>
+        <v>2608</v>
       </c>
       <c r="D3" s="4">
-        <v>561.0</v>
+        <v>561</v>
       </c>
       <c r="E3" s="4">
-        <v>559.0</v>
+        <v>559</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -600,55 +640,55 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="6">
+    <row r="6" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7">
+    <row r="7" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8">
+    <row r="8" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="12">
-        <v>768.0</v>
+        <v>768</v>
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9">
+    <row r="9" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="14">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10">
+    <row r="10" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="14">
-        <v>256.0</v>
+        <v>256</v>
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11">
+    <row r="11" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="14">
-        <v>128.0</v>
+        <v>128</v>
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
@@ -657,7 +697,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13">
+    <row r="13" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
@@ -666,26 +706,26 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14">
+    <row r="14" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="16">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="9"/>
     </row>
-    <row r="15">
+    <row r="15" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16">
+    <row r="16" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>17</v>
       </c>
@@ -696,63 +736,63 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="18">
-        <v>0.709507042253521</v>
+        <v>0.70950704225352101</v>
       </c>
       <c r="D18" s="19">
-        <v>0.708928571428571</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>0.70892857142857102</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="18">
-        <v>0.700704225352112</v>
+        <v>0.70070422535211196</v>
       </c>
       <c r="D19" s="19">
-        <v>0.721173469387755</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0.72117346938775495</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="20">
-        <v>0.691901408450704</v>
+        <v>0.69190140845070403</v>
       </c>
       <c r="D20" s="21">
-        <v>0.69438775510204</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0.69438775510203998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="22">
-        <v>0.697183098591549</v>
+        <v>0.69718309859154903</v>
       </c>
       <c r="D21" s="23">
-        <v>0.698214285714285</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>0.69821428571428501</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-    </row>
-    <row r="25">
+      <c r="C22" s="18"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="25" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>25</v>
       </c>
@@ -763,88 +803,412 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="18"/>
       <c r="D26" s="19"/>
     </row>
-    <row r="27">
+    <row r="27" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="18"/>
       <c r="D27" s="19"/>
     </row>
-    <row r="28">
+    <row r="28" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
     </row>
-    <row r="29">
+    <row r="29" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
       <c r="C29" s="22"/>
       <c r="D29" s="23"/>
     </row>
-    <row r="30">
+    <row r="30" spans="2:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="28"/>
-      <c r="S33" s="28"/>
-      <c r="T33" s="28"/>
-      <c r="U33" s="28"/>
-      <c r="V33" s="28"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
-      <c r="Y33" s="28"/>
-      <c r="Z33" s="28"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="24"/>
+    </row>
+    <row r="33" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="56.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2608</v>
+      </c>
+      <c r="D3" s="4">
+        <v>561</v>
+      </c>
+      <c r="E3" s="4">
+        <v>559</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="6" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12">
+        <v>768</v>
+      </c>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14">
+        <v>100</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14">
+        <v>256</v>
+      </c>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="14">
+        <v>128</v>
+      </c>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="16">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="31">
+        <v>768</v>
+      </c>
+      <c r="G18" s="32">
+        <v>300</v>
+      </c>
+      <c r="H18" s="32">
+        <v>100</v>
+      </c>
+      <c r="I18" s="32">
+        <v>256</v>
+      </c>
+      <c r="J18" s="32">
+        <v>128</v>
+      </c>
+      <c r="K18" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="M18" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B21" s="11"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="24"/>
+    </row>
+    <row r="23" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+    </row>
+    <row r="25" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B26" s="11"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="2:13" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="24"/>
+    </row>
+    <row r="33" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>